<commit_message>
define knowledge types for edge skill perreqs
</commit_message>
<xml_diff>
--- a/docs/edges/edges.xlsx
+++ b/docs/edges/edges.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdavis\IdeaProjects\srg\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7935" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="defs" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="attr_prereq" sheetId="3" r:id="rId4"/>
     <sheet name="skill_prereq" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1553,7 +1548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4804,7 +4799,7 @@
 SET @BURN_FOR_GLORY_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>280</v>
       </c>
@@ -4832,7 +4827,7 @@
 SET @BURN_PAST_THE_PAIN_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>281</v>
       </c>
@@ -4860,7 +4855,7 @@
 SET @BURN_FOR_TOMORROW_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>282</v>
       </c>
@@ -4916,7 +4911,7 @@
 SET @IMPROVED_CYBERKINETIC_AWARENESS_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>284</v>
       </c>
@@ -4944,7 +4939,7 @@
 SET @CYBERKINETIC_DENIAL_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>285</v>
       </c>
@@ -4972,7 +4967,7 @@
 SET @FLAME_BLAST_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>286</v>
       </c>
@@ -5112,7 +5107,7 @@
 SET @MASTER_CYBER_ARMOR_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>291</v>
       </c>
@@ -5140,7 +5135,7 @@
 SET @IMPROVED_FIERY_AURA_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>292</v>
       </c>
@@ -5168,7 +5163,7 @@
 SET @IMPROVED_FIRE_MASTERY_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>293</v>
       </c>
@@ -5280,7 +5275,7 @@
 SET @MASTER_PSI_SWORD_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>297</v>
       </c>
@@ -5308,7 +5303,7 @@
 SET @LEY_LINE_OBSERVATION_SPHERE_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>298</v>
       </c>
@@ -5364,7 +5359,7 @@
 SET @LEY_LINE_GATE_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>300</v>
       </c>
@@ -5392,7 +5387,7 @@
 SET @OFF_THE_HANDLE_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>301</v>
       </c>
@@ -5448,7 +5443,7 @@
 SET @RAPID_FLAME_BOLT_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>303</v>
       </c>
@@ -5532,7 +5527,7 @@
 SET @BURN_FASTER_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>306</v>
       </c>
@@ -5560,7 +5555,7 @@
 SET @SUBLIME_CHAOS_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>307</v>
       </c>
@@ -5812,7 +5807,7 @@
 SET @TRICKY_FIGHTER_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>316</v>
       </c>
@@ -5868,7 +5863,7 @@
 SET @IMPROVED_CYBER_PSYCHIC_ALIGNMENT_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>318</v>
       </c>
@@ -5899,7 +5894,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>319</v>
       </c>
@@ -6045,7 +6040,7 @@
 SET @COMBAT_ACE_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>324</v>
       </c>
@@ -6185,7 +6180,7 @@
 SET @ROBOT_ARMOR_JOCK_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>329</v>
       </c>
@@ -6213,7 +6208,7 @@
 SET @I_KNOW_A_GUY_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>330</v>
       </c>
@@ -6260,7 +6255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -8840,10 +8835,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E62" sqref="E2:E62"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8851,10 +8846,11 @@
     <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="133" customWidth="1"/>
+    <col min="5" max="5" width="114.42578125" customWidth="1"/>
+    <col min="6" max="6" width="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>237</v>
       </c>
@@ -8868,7 +8864,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -8883,7 +8879,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@BLOCK_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -8898,7 +8894,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@COUNTERATTACK_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -8913,7 +8909,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@FLORENTINE_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -8928,7 +8924,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@FRENZY_ID, 'FIGHTING', 'D10');</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -8943,7 +8939,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MARTIAL_ARTIST_ID, 'FIGHTING', 'D6');</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -8958,7 +8954,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@IMPROVED_MARTIAL_ARTIST_ID, 'FIGHTING', 'D10');</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -8973,7 +8969,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ROCK_AND_ROLL_ID, 'SHOOTING', 'D8');</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -8988,7 +8984,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@SWEEP_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -9003,7 +8999,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@TRADEMARK_WEAPON_ID, 'FIGHTING', 'D10');</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -9018,7 +9014,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@TRADEMARK_WEAPON_ID, 'SHOOTING', 'D10');</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -9035,8 +9031,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@TACTICIAN_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f>"UPDATE `edge_skill_prerequisite` SET skill_knowledge = @"&amp;D12&amp;"_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = '"&amp;A12&amp;"');"</f>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @BATTLE_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'TACTICIAN');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -9053,8 +9053,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@SOUL_DRAIN_ID, 'KNOWLEDGE', 'D10');</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f>"UPDATE `edge_skill_prerequisite` SET skill_knowledge = @"&amp;D13&amp;"_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = '"&amp;A13&amp;"');"</f>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ARCANA_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'SOUL_DRAIN');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -9069,7 +9073,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ADEPT_ID, 'FAITH', 'D8');</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -9084,7 +9088,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ADEPT_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -9099,7 +9103,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ASSASSIN_ID, 'CLIMBING', 'D6');</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -9114,7 +9118,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ASSASSIN_ID, 'FIGHTING', 'D6');</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -9129,7 +9133,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ASSASSIN_ID, 'STEALTH', 'D8');</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -9144,7 +9148,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@CHAMPION_ID, 'FAITH', 'D6');</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -9159,7 +9163,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@CHAMPION_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -9174,7 +9178,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@GADGETEER_ID, 'WEIRD_SCIENCE', 'D8');</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -9191,8 +9195,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@GADGETEER_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" ref="F14:F58" si="1">"UPDATE `edge_skill_prerequisite` SET skill_knowledge = @"&amp;D22&amp;"_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = '"&amp;A22&amp;"');"</f>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ANY_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'GADGETEER');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -9209,8 +9217,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@GADGETEER_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ANY_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'GADGETEER');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -9225,7 +9237,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@HOLY_UNHOLY_WARRIOR_ID, 'FAITH', 'D6');</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -9240,7 +9252,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@INVESTIGATOR_ID, 'INVESTIGATION', 'D8');</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -9255,7 +9267,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@INVESTIGATOR_ID, 'STREETWISE', 'D8');</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -9270,7 +9282,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MCGUYVER_ID, 'REPAIR', 'D6');</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -9285,7 +9297,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MCGUYVER_ID, 'NOTICE', 'D8');</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -9300,7 +9312,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MENTALIST_ID, 'PSIONICS', 'D6');</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -9315,7 +9327,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MR_FIX_IT_ID, 'REPAIR', 'D8');</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -9330,7 +9342,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MR_FIX_IT_ID, 'WEIRD_SCIENCE', 'D8');</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -9347,8 +9359,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MR_FIX_IT_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ANY_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'MR_FIX_IT');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -9365,8 +9381,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MR_FIX_IT_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ANY_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'MR_FIX_IT');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -9381,7 +9401,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@THIEF_ID, 'CLIMBING', 'D6');</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -9396,7 +9416,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@THIEF_ID, 'LOCKPICKING', 'D6');</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -9411,7 +9431,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@THIEF_ID, 'STEALTH', 'D8');</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -9428,8 +9448,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@WIZARD_ID, 'KNOWLEDGE', 'D8');</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ARCANA_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'WIZARD');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -9444,7 +9468,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@WIZARD_ID, 'SPELLCASTING', 'D6');</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -9459,7 +9483,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@WOODSMAN_ID, 'SURVIVAL', 'D8');</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -9474,7 +9498,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@WOODSMAN_ID, 'TRACKING', 'D8');</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -9489,7 +9513,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@STRONG_WILLED_ID, 'INTIMIDATION', 'D6');</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -9504,7 +9528,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@STRONG_WILLED_ID, 'TAUNT', 'D6');</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -9519,7 +9543,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MARTIAL_ARTS_MASTER_ID, 'FIGHTING', 'D12');</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -9534,10 +9558,10 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@WEAPON_MASTER_ID, 'FIGHTING', 'D12');</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>282</v>
       </c>
@@ -9552,7 +9576,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@CYBERKINETIC_AWARENESS_ID, 'NOTICE', 'D6');</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>283</v>
       </c>
@@ -9567,7 +9591,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@IMPROVED_CYBERKINETIC_AWARENESS_ID, 'NOTICE', 'D8');</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>287</v>
       </c>
@@ -9582,7 +9606,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@GUN_NUT_ID, 'SHOOTING', 'D8');</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>288</v>
       </c>
@@ -9597,7 +9621,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@GYMNASTIC_MASTERY_ID, 'CLIMBING', 'D6');</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>303</v>
       </c>
@@ -9612,7 +9636,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@READ_THE_FLAME_ID, 'NOTICE', 'D6');</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>310</v>
       </c>
@@ -9627,7 +9651,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@CHARGE_ID, 'FIGHTING', 'D10');</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>312</v>
       </c>
@@ -9642,7 +9666,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@COMBAT_SENSE_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>312</v>
       </c>
@@ -9657,7 +9681,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@COMBAT_SENSE_ID, 'NOTICE', 'D8');</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>315</v>
       </c>
@@ -9672,7 +9696,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@TRICKY_FIGHTER_ID, 'FIGHTING', 'D8');</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>324</v>
       </c>
@@ -9687,7 +9711,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MAJOR_PSIONIC_ID, 'PSIONICS', 'D8');</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>325</v>
       </c>
@@ -9702,7 +9726,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MASTER_PSIONIC_ID, 'PSIONICS', 'D10');</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>326</v>
       </c>
@@ -9717,7 +9741,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MASTER_OF_MAGIC_ID, 'ARCANA', 'D8');</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>326</v>
       </c>
@@ -9734,8 +9758,12 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@MASTER_OF_MAGIC_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ARCANA_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'MASTER_OF_MAGIC');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>328</v>
       </c>
@@ -9750,7 +9778,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@ROBOT_ARMOR_JOCK_ID, 'PILOTING', 'D6');</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>329</v>
       </c>
@@ -9765,7 +9793,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@I_KNOW_A_GUY_ID, 'PERSUASION', 'D6');</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>329</v>
       </c>
@@ -9780,7 +9808,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@I_KNOW_A_GUY_ID, 'STREETWISE', 'D6');</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>330</v>
       </c>

</xml_diff>

<commit_message>
edge purchase working, some ui fixes, started converting some enum types to serialize as objects
</commit_message>
<xml_diff>
--- a/docs/edges/edges.xlsx
+++ b/docs/edges/edges.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdavis\IdeaProjects\srg\docs\edges\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7935" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="defs" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="attr_prereq" sheetId="3" r:id="rId4"/>
     <sheet name="skill_prereq" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1548,7 +1553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1558,9 +1563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H114" sqref="H114:H167"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3376,7 +3381,7 @@
         <v>111</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>180</v>
@@ -3392,7 +3397,7 @@
       </c>
       <c r="H65" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `edge` (edge_type, edge_category_type, xp_level_type, description, attribute_prerequisite_logic_type, skill_prerequisite_logic_type, edge_prerequisite_logic_type) VALUES ('INSPIRE', 'LEADERSHIP', 'INSPIRE', 'Leaders with exceptional reputations and experience in battle inspire the soldiers around them. They add +2 to Spirit rolls when recovering from being Shaken (this includes the original +1 bonus for the Command Edge). ', 'OR', 'OR', 'OR');
+        <v>INSERT INTO `edge` (edge_type, edge_category_type, xp_level_type, description, attribute_prerequisite_logic_type, skill_prerequisite_logic_type, edge_prerequisite_logic_type) VALUES ('INSPIRE', 'LEADERSHIP', 'SEASONED', 'Leaders with exceptional reputations and experience in battle inspire the soldiers around them. They add +2 to Spirit rolls when recovering from being Shaken (this includes the original +1 bonus for the Command Edge). ', 'OR', 'OR', 'OR');
 SET @INSPIRE_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
@@ -8837,7 +8842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+    <sheetView topLeftCell="D37" workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
@@ -9196,7 +9201,7 @@
         <v>INSERT INTO `edge_skill_prerequisite` (edge, skill_type, die_type) VALUES (@GADGETEER_ID, 'KNOWLEDGE', 'D6');</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ref="F14:F58" si="1">"UPDATE `edge_skill_prerequisite` SET skill_knowledge = @"&amp;D22&amp;"_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = '"&amp;A22&amp;"');"</f>
+        <f t="shared" ref="F22:F58" si="1">"UPDATE `edge_skill_prerequisite` SET skill_knowledge = @"&amp;D22&amp;"_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = '"&amp;A22&amp;"');"</f>
         <v>UPDATE `edge_skill_prerequisite` SET skill_knowledge = @ANY_ID WHERE edge = (SELECT id FROM `edge` WHERE edge_type = 'GADGETEER');</v>
       </c>
     </row>

</xml_diff>